<commit_message>
changed resistor value and pcb
</commit_message>
<xml_diff>
--- a/Temp_Amp_01/Release/BOM/Bill of Materials-TEMP_SENS_1.xlsx
+++ b/Temp_Amp_01/Release/BOM/Bill of Materials-TEMP_SENS_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -36,7 +36,7 @@
     <t>CAP CER 0.1UF 16V X7R 0603</t>
   </si>
   <si>
-    <t>C1</t>
+    <t>C1, C4</t>
   </si>
   <si>
     <t>C0603C104M4RACTU</t>
@@ -51,15 +51,6 @@
     <t>C0603C105K4RACTU</t>
   </si>
   <si>
-    <t>CAP CER 0.068UF 16V X7R 0603</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>CC0603KRX7R7BB683</t>
-  </si>
-  <si>
     <t>THERMOPILE IR SENSOR with thermistor</t>
   </si>
   <si>
@@ -72,12 +63,6 @@
     <t>JP1</t>
   </si>
   <si>
-    <t>Single layer pad TP</t>
-  </si>
-  <si>
-    <t>JP2 Vref, JP3 Vout</t>
-  </si>
-  <si>
     <t>Mounting hole, 4.2mm</t>
   </si>
   <si>
@@ -105,13 +90,10 @@
     <t>CRCW06031K00FKEA</t>
   </si>
   <si>
-    <t>RES SMD 49.9K OHM 1% 1/10W 0603</t>
+    <t>RES SMD 200K OHM 1% 1/10W 0603</t>
   </si>
   <si>
     <t>R4</t>
-  </si>
-  <si>
-    <t>RC0603FR-0749K9L</t>
   </si>
   <si>
     <t>RES SMD 75K OHM 1% 1/8W 0603</t>
@@ -464,7 +446,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -498,7 +480,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="46" t="s">
         <v>7</v>
@@ -528,16 +510,14 @@
       <c r="C4" s="50">
         <v>1</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>13</v>
-      </c>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>15</v>
       </c>
       <c r="C5" s="50">
         <v>1</v>
@@ -546,51 +526,53 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="49" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="49" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="49" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="49"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="C9" s="50">
+        <v>1</v>
+      </c>
+      <c r="D9" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="50">
-        <v>1</v>
-      </c>
-      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="48" t="s">
@@ -614,47 +596,19 @@
       <c r="C11" s="50">
         <v>1</v>
       </c>
-      <c r="D11" s="49" t="s">
-        <v>28</v>
-      </c>
+      <c r="D11" s="49"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="49" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" s="50">
         <v>1</v>
       </c>
-      <c r="D12" s="49" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="50">
-        <v>1</v>
-      </c>
-      <c r="D13" s="49"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="50">
-        <v>1</v>
-      </c>
-      <c r="D14" s="49"/>
+      <c r="D12" s="49"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
changed to vertical headers and added TP
</commit_message>
<xml_diff>
--- a/Temp_Amp_01/Release/BOM/Bill of Materials-TEMP_SENS_1.xlsx
+++ b/Temp_Amp_01/Release/BOM/Bill of Materials-TEMP_SENS_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Description</t>
   </si>
@@ -57,10 +57,16 @@
     <t>IR1</t>
   </si>
   <si>
-    <t>CONN HEADER R/A 3POS 1.25MM</t>
+    <t>CONN HEADER VERT 3POS 2.54MM</t>
   </si>
   <si>
     <t>JP1</t>
+  </si>
+  <si>
+    <t>Single layer pad TP</t>
+  </si>
+  <si>
+    <t>JP2, JP3</t>
   </si>
   <si>
     <t>Mounting hole, 4.2mm</t>
@@ -446,7 +452,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -544,7 +550,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="49"/>
     </row>
@@ -570,21 +576,21 @@
       <c r="C9" s="50">
         <v>1</v>
       </c>
-      <c r="D9" s="49" t="s">
-        <v>23</v>
-      </c>
+      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="C10" s="50">
+        <v>1</v>
+      </c>
+      <c r="D10" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="50">
-        <v>1</v>
-      </c>
-      <c r="D10" s="49"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="48" t="s">
@@ -609,6 +615,18 @@
         <v>1</v>
       </c>
       <c r="D12" s="49"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="50">
+        <v>1</v>
+      </c>
+      <c r="D13" s="49"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>